<commit_message>
Flere figurer + nyt katalog: categoryexperiment (ID og EOP)
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/Othdata_main_catalog.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>26</v>
       </c>
       <c r="G2">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>26</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>26</v>
       </c>
       <c r="C7">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +605,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +663,7 @@
         <v>23</v>
       </c>
       <c r="E4">
-        <v>0.25</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
pre merge (merger igen)
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_main_catalog.xlsx
+++ b/examples/Abatement/Data/Othdata_main_catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>